<commit_message>
Cleanup, distance-radius tranisiton, and data out
Cleanup from miscellaneous troubleshooting. Changed from a lat/lon
degree-radius distance to pixel scaled to distance radius. Refined plume
troubleshooting NetCDF output file/directory scheme, and began ability
to output stats to CSV file.
</commit_message>
<xml_diff>
--- a/SatelliteList.xlsx
+++ b/SatelliteList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danp/Desktop/CAUrbanRunoffPlumes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD538C-D70F-5B42-A9EF-088630A4E22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2772C469-8381-EA4C-BEC8-C440CA972F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5980" yWindow="2800" windowWidth="27240" windowHeight="16440" xr2:uid="{C42C0B04-E0B6-DF4C-9883-029DD1464C52}"/>
   </bookViews>

</xml_diff>